<commit_message>
Updated until end of June
</commit_message>
<xml_diff>
--- a/data/special_days.xlsx
+++ b/data/special_days.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Manue\Documents\R Scripts\Catholic_Calendar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA59F5EE-6249-4CF5-AB67-48181C6AC490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3681BA2-6D44-46AF-A529-ED8BF567B201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{DB0BE976-C12D-413B-BEEB-3B29EA804A45}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
   <si>
     <t>type</t>
   </si>
@@ -90,6 +90,90 @@
   </si>
   <si>
     <t>day</t>
+  </si>
+  <si>
+    <t>Darstellung des Herrn</t>
+  </si>
+  <si>
+    <t>Agatha</t>
+  </si>
+  <si>
+    <t>Paul Miki und Gefährten</t>
+  </si>
+  <si>
+    <t>Scholastika</t>
+  </si>
+  <si>
+    <t>Cyrill und Methodius Slawenmission</t>
+  </si>
+  <si>
+    <t>Kathedra Petri</t>
+  </si>
+  <si>
+    <t>Polykarp</t>
+  </si>
+  <si>
+    <t>Matthias (Apstl.)</t>
+  </si>
+  <si>
+    <t>Perpetua und Felizitas</t>
+  </si>
+  <si>
+    <t>Josef, Bräutigam der Gottesmutter Maria</t>
+  </si>
+  <si>
+    <t>Verkündigung des Herrn</t>
+  </si>
+  <si>
+    <t>Johannes Baptist de la Salle</t>
+  </si>
+  <si>
+    <t>Stanislaus</t>
+  </si>
+  <si>
+    <t>Markus (Evgl.)</t>
+  </si>
+  <si>
+    <t>Katharina von Siena</t>
+  </si>
+  <si>
+    <t>Athanasius</t>
+  </si>
+  <si>
+    <t>Philippus und Jakobus (Apstl.)</t>
+  </si>
+  <si>
+    <t>Christophorus Magallanes und Hermann Josef</t>
+  </si>
+  <si>
+    <t>Philipp Neri</t>
+  </si>
+  <si>
+    <t>Justin</t>
+  </si>
+  <si>
+    <t>Karl Lwanga und Gefährten</t>
+  </si>
+  <si>
+    <t>Bonifatius</t>
+  </si>
+  <si>
+    <t>Barnabas (Apstl.)</t>
+  </si>
+  <si>
+    <t>Antonius von Padua</t>
+  </si>
+  <si>
+    <t>Aloisius Gonzaga</t>
+  </si>
+  <si>
+    <t>Geburt Johannes des Täufers</t>
+  </si>
+  <si>
+    <t>Irenäus</t>
+  </si>
+  <si>
+    <t>Petrus und Paulus (Apstl.)</t>
   </si>
 </sst>
 </file>
@@ -453,11 +537,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AE50AD-9324-4F6C-B024-445672FDC880}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -624,6 +706,398 @@
         <v>13</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>2</v>
+      </c>
+      <c r="B12" s="4">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>2</v>
+      </c>
+      <c r="B13" s="4">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>2</v>
+      </c>
+      <c r="B14" s="4">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>2</v>
+      </c>
+      <c r="B15" s="4">
+        <v>10</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>2</v>
+      </c>
+      <c r="B16" s="4">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>2</v>
+      </c>
+      <c r="B17" s="4">
+        <v>22</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>2</v>
+      </c>
+      <c r="B18" s="4">
+        <v>23</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>2</v>
+      </c>
+      <c r="B19" s="4">
+        <v>24</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>3</v>
+      </c>
+      <c r="B20" s="4">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>3</v>
+      </c>
+      <c r="B21" s="4">
+        <v>19</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>3</v>
+      </c>
+      <c r="B22" s="4">
+        <v>25</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>4</v>
+      </c>
+      <c r="B23" s="4">
+        <v>7</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>4</v>
+      </c>
+      <c r="B24" s="4">
+        <v>11</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>4</v>
+      </c>
+      <c r="B25" s="4">
+        <v>25</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>4</v>
+      </c>
+      <c r="B26" s="4">
+        <v>29</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>5</v>
+      </c>
+      <c r="B27" s="4">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>5</v>
+      </c>
+      <c r="B28" s="4">
+        <v>3</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>5</v>
+      </c>
+      <c r="B29" s="4">
+        <v>21</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>5</v>
+      </c>
+      <c r="B30" s="4">
+        <v>26</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>6</v>
+      </c>
+      <c r="B31" s="4">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>6</v>
+      </c>
+      <c r="B32" s="4">
+        <v>3</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>6</v>
+      </c>
+      <c r="B33" s="4">
+        <v>5</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>6</v>
+      </c>
+      <c r="B34" s="4">
+        <v>11</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>6</v>
+      </c>
+      <c r="B35" s="4">
+        <v>13</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>6</v>
+      </c>
+      <c r="B36" s="4">
+        <v>21</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>6</v>
+      </c>
+      <c r="B37" s="4">
+        <v>24</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>6</v>
+      </c>
+      <c r="B38" s="4">
+        <v>28</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>6</v>
+      </c>
+      <c r="B39" s="4">
+        <v>29</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Preliminarily finished, leap_year prcedure needs to be fixed
</commit_message>
<xml_diff>
--- a/data/special_days.xlsx
+++ b/data/special_days.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Manue\Documents\R Scripts\Catholic_Calendar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3681BA2-6D44-46AF-A529-ED8BF567B201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBD19DE-ED3C-431F-9403-2651B8D6F7E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{DB0BE976-C12D-413B-BEEB-3B29EA804A45}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="113">
   <si>
     <t>type</t>
   </si>
@@ -174,6 +174,207 @@
   </si>
   <si>
     <t>Petrus und Paulus (Apstl.)</t>
+  </si>
+  <si>
+    <t>Mariä Heimsuchung</t>
+  </si>
+  <si>
+    <t>Thomas (Apstl.)</t>
+  </si>
+  <si>
+    <t>Benedikt von Nursia</t>
+  </si>
+  <si>
+    <t>Bonaventura</t>
+  </si>
+  <si>
+    <t>Maria Magdalena</t>
+  </si>
+  <si>
+    <t>Birgitta von Schweden</t>
+  </si>
+  <si>
+    <t>Jakobus (Apstl.)</t>
+  </si>
+  <si>
+    <t>Joachim und Anna</t>
+  </si>
+  <si>
+    <t>Martha, Maria und Lazarus</t>
+  </si>
+  <si>
+    <t>Ignatius von Loyola</t>
+  </si>
+  <si>
+    <t>Alfons Maria von Liguori</t>
+  </si>
+  <si>
+    <t>Johannes Maria Vianney</t>
+  </si>
+  <si>
+    <t>Verklärung des Herrn</t>
+  </si>
+  <si>
+    <t>Dominikus</t>
+  </si>
+  <si>
+    <t>Edith Stein</t>
+  </si>
+  <si>
+    <t>Laurentius</t>
+  </si>
+  <si>
+    <t>Klara von Assisi</t>
+  </si>
+  <si>
+    <t>Maximilian Kolbe</t>
+  </si>
+  <si>
+    <t>Mariä Aufnahme in den Himmel</t>
+  </si>
+  <si>
+    <t>Bernhard von Clairvaux</t>
+  </si>
+  <si>
+    <t>Pius X</t>
+  </si>
+  <si>
+    <t>Maria Königin</t>
+  </si>
+  <si>
+    <t>Bartholomäus</t>
+  </si>
+  <si>
+    <t>Monika</t>
+  </si>
+  <si>
+    <t>Augustinus</t>
+  </si>
+  <si>
+    <t>Enthauptung Johannes' des Täufers</t>
+  </si>
+  <si>
+    <t>Gregor der Große</t>
+  </si>
+  <si>
+    <t>Teresa von Kalkutta</t>
+  </si>
+  <si>
+    <t>Mariä Geburt</t>
+  </si>
+  <si>
+    <t>Johannes Chrysostomus</t>
+  </si>
+  <si>
+    <t>Kreuzerhöhung</t>
+  </si>
+  <si>
+    <t>Gedächtnis der Schmerzen Mariens</t>
+  </si>
+  <si>
+    <t>Kornelius unc Cyprian</t>
+  </si>
+  <si>
+    <t>Andreas Kim Taegon</t>
+  </si>
+  <si>
+    <t>Matthäus (Apstl. und Evgl.)</t>
+  </si>
+  <si>
+    <t>Vinzenz von Paul</t>
+  </si>
+  <si>
+    <t>Michael, Gabriel und Rafael</t>
+  </si>
+  <si>
+    <t>Hieronymus</t>
+  </si>
+  <si>
+    <t>Theresia vom Kinde Jesus</t>
+  </si>
+  <si>
+    <t>Schutzengel</t>
+  </si>
+  <si>
+    <t>Franz von Assisi</t>
+  </si>
+  <si>
+    <t>Gedenktag Unserer Lieben Frau vom Rosenkranz</t>
+  </si>
+  <si>
+    <t>Theresia von Avila</t>
+  </si>
+  <si>
+    <t>Ignatius</t>
+  </si>
+  <si>
+    <t>Lukas (Evgl.)</t>
+  </si>
+  <si>
+    <t>Simon und Judas (Apstl.)</t>
+  </si>
+  <si>
+    <t>Allerheiligen</t>
+  </si>
+  <si>
+    <t>Allerseelen</t>
+  </si>
+  <si>
+    <t>Karl Borromäus</t>
+  </si>
+  <si>
+    <t>Weihetag der Lateranbasilika</t>
+  </si>
+  <si>
+    <t>Leo der Große</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Josaphat</t>
+  </si>
+  <si>
+    <t>Elisabeth</t>
+  </si>
+  <si>
+    <t>Gedenktag Unserer Lieben Frau in Jerusalem</t>
+  </si>
+  <si>
+    <t>Cäcilia</t>
+  </si>
+  <si>
+    <t>Andreas Dung-Lac</t>
+  </si>
+  <si>
+    <t>Andreas (Apstl.)</t>
+  </si>
+  <si>
+    <t>Franz Xaver</t>
+  </si>
+  <si>
+    <t>Ambrosius</t>
+  </si>
+  <si>
+    <t>Hochfest der ohne Erbsünde empfangenen Jungfrau und Gottesmutter Maria</t>
+  </si>
+  <si>
+    <t>Juan Diego</t>
+  </si>
+  <si>
+    <t>Johannes vom Kreuz</t>
+  </si>
+  <si>
+    <t>Hochfest der Geburt des Herrn - Weihnachten</t>
+  </si>
+  <si>
+    <t>Stephanus</t>
+  </si>
+  <si>
+    <t>Johannes (Apstl. und Evgl.)</t>
+  </si>
+  <si>
+    <t>Unschuldige Kinder</t>
   </si>
 </sst>
 </file>
@@ -537,7 +738,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AE50AD-9324-4F6C-B024-445672FDC880}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -545,8 +746,8 @@
   <cols>
     <col min="1" max="2" width="10.7109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="45.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="45.7109375" customWidth="1"/>
+    <col min="4" max="4" width="70.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="70.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1098,6 +1299,944 @@
         <v>45</v>
       </c>
     </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>7</v>
+      </c>
+      <c r="B40" s="4">
+        <v>2</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>7</v>
+      </c>
+      <c r="B41" s="4">
+        <v>3</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>7</v>
+      </c>
+      <c r="B42" s="4">
+        <v>11</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>7</v>
+      </c>
+      <c r="B43" s="4">
+        <v>15</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>7</v>
+      </c>
+      <c r="B44" s="4">
+        <v>22</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>7</v>
+      </c>
+      <c r="B45" s="4">
+        <v>23</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>7</v>
+      </c>
+      <c r="B46" s="4">
+        <v>25</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>7</v>
+      </c>
+      <c r="B47" s="4">
+        <v>25</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>7</v>
+      </c>
+      <c r="B48" s="4">
+        <v>29</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>7</v>
+      </c>
+      <c r="B49" s="4">
+        <v>31</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>8</v>
+      </c>
+      <c r="B50" s="4">
+        <v>1</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>8</v>
+      </c>
+      <c r="B51" s="4">
+        <v>4</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>8</v>
+      </c>
+      <c r="B52" s="4">
+        <v>6</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>8</v>
+      </c>
+      <c r="B53" s="4">
+        <v>8</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>8</v>
+      </c>
+      <c r="B54" s="4">
+        <v>9</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>8</v>
+      </c>
+      <c r="B55" s="4">
+        <v>10</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <v>8</v>
+      </c>
+      <c r="B56" s="4">
+        <v>11</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
+        <v>8</v>
+      </c>
+      <c r="B57" s="4">
+        <v>14</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
+        <v>8</v>
+      </c>
+      <c r="B58" s="4">
+        <v>15</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
+        <v>8</v>
+      </c>
+      <c r="B59" s="4">
+        <v>20</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
+        <v>8</v>
+      </c>
+      <c r="B60" s="4">
+        <v>21</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="4">
+        <v>8</v>
+      </c>
+      <c r="B61" s="4">
+        <v>22</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="4">
+        <v>8</v>
+      </c>
+      <c r="B62" s="4">
+        <v>24</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="4">
+        <v>8</v>
+      </c>
+      <c r="B63" s="4">
+        <v>27</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="4">
+        <v>8</v>
+      </c>
+      <c r="B64" s="4">
+        <v>28</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="4">
+        <v>8</v>
+      </c>
+      <c r="B65" s="4">
+        <v>29</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="4">
+        <v>9</v>
+      </c>
+      <c r="B66" s="4">
+        <v>3</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="4">
+        <v>9</v>
+      </c>
+      <c r="B67" s="4">
+        <v>5</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="4">
+        <v>9</v>
+      </c>
+      <c r="B68" s="4">
+        <v>8</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="4">
+        <v>9</v>
+      </c>
+      <c r="B69" s="4">
+        <v>13</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="4">
+        <v>9</v>
+      </c>
+      <c r="B70" s="4">
+        <v>14</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="4">
+        <v>9</v>
+      </c>
+      <c r="B71" s="4">
+        <v>15</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="4">
+        <v>9</v>
+      </c>
+      <c r="B72" s="4">
+        <v>16</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="4">
+        <v>9</v>
+      </c>
+      <c r="B73" s="4">
+        <v>20</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <v>9</v>
+      </c>
+      <c r="B74" s="4">
+        <v>21</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="4">
+        <v>9</v>
+      </c>
+      <c r="B75" s="4">
+        <v>27</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="4">
+        <v>9</v>
+      </c>
+      <c r="B76" s="4">
+        <v>29</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="4">
+        <v>9</v>
+      </c>
+      <c r="B77" s="4">
+        <v>30</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="4">
+        <v>10</v>
+      </c>
+      <c r="B78" s="4">
+        <v>1</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="4">
+        <v>10</v>
+      </c>
+      <c r="B79" s="4">
+        <v>2</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="4">
+        <v>10</v>
+      </c>
+      <c r="B80" s="4">
+        <v>4</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="4">
+        <v>10</v>
+      </c>
+      <c r="B81" s="4">
+        <v>7</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="4">
+        <v>10</v>
+      </c>
+      <c r="B82" s="4">
+        <v>15</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="4">
+        <v>10</v>
+      </c>
+      <c r="B83" s="4">
+        <v>17</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="4">
+        <v>10</v>
+      </c>
+      <c r="B84" s="4">
+        <v>18</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="4">
+        <v>10</v>
+      </c>
+      <c r="B85" s="4">
+        <v>28</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="4">
+        <v>11</v>
+      </c>
+      <c r="B86" s="4">
+        <v>1</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="4">
+        <v>11</v>
+      </c>
+      <c r="B87" s="4">
+        <v>2</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="4">
+        <v>11</v>
+      </c>
+      <c r="B88" s="4">
+        <v>4</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="4">
+        <v>11</v>
+      </c>
+      <c r="B89" s="4">
+        <v>9</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="4">
+        <v>11</v>
+      </c>
+      <c r="B90" s="4">
+        <v>10</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="4">
+        <v>11</v>
+      </c>
+      <c r="B91" s="4">
+        <v>11</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="4">
+        <v>11</v>
+      </c>
+      <c r="B92" s="4">
+        <v>12</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="4">
+        <v>11</v>
+      </c>
+      <c r="B93" s="4">
+        <v>19</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="4">
+        <v>11</v>
+      </c>
+      <c r="B94" s="4">
+        <v>21</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="4">
+        <v>11</v>
+      </c>
+      <c r="B95" s="4">
+        <v>22</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="4">
+        <v>11</v>
+      </c>
+      <c r="B96" s="4">
+        <v>24</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="4">
+        <v>11</v>
+      </c>
+      <c r="B97" s="4">
+        <v>30</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="4">
+        <v>12</v>
+      </c>
+      <c r="B98" s="4">
+        <v>3</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="4">
+        <v>12</v>
+      </c>
+      <c r="B99" s="4">
+        <v>7</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="4">
+        <v>12</v>
+      </c>
+      <c r="B100" s="4">
+        <v>8</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="4">
+        <v>12</v>
+      </c>
+      <c r="B101" s="4">
+        <v>9</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="4">
+        <v>12</v>
+      </c>
+      <c r="B102" s="4">
+        <v>14</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="4">
+        <v>12</v>
+      </c>
+      <c r="B103" s="4">
+        <v>25</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="4">
+        <v>12</v>
+      </c>
+      <c r="B104" s="4">
+        <v>26</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="4">
+        <v>12</v>
+      </c>
+      <c r="B105" s="4">
+        <v>27</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="4">
+        <v>12</v>
+      </c>
+      <c r="B106" s="4">
+        <v>28</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added martyr field, started on colours
</commit_message>
<xml_diff>
--- a/data/special_days.xlsx
+++ b/data/special_days.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Manue\Documents\R Scripts\Catholic_Calendar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBD19DE-ED3C-431F-9403-2651B8D6F7E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D205148-71FF-4BAD-91C0-8E0819E4374E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{DB0BE976-C12D-413B-BEEB-3B29EA804A45}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="115">
   <si>
     <t>type</t>
   </si>
@@ -375,6 +375,12 @@
   </si>
   <si>
     <t>Unschuldige Kinder</t>
+  </si>
+  <si>
+    <t>is_martyr</t>
+  </si>
+  <si>
+    <t>TRUE</t>
   </si>
 </sst>
 </file>
@@ -418,12 +424,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,19 +747,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AE50AD-9324-4F6C-B024-445672FDC880}">
-  <dimension ref="A1:E106"/>
+  <dimension ref="A1:F106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="10.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="70.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="70.7109375" customWidth="1"/>
+    <col min="3" max="4" width="20.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="70.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="70.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -761,13 +770,16 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -777,11 +789,14 @@
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -791,11 +806,14 @@
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -805,11 +823,14 @@
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -819,11 +840,14 @@
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -833,11 +857,14 @@
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>1</v>
       </c>
@@ -847,11 +874,14 @@
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>1</v>
       </c>
@@ -861,11 +891,14 @@
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -875,11 +908,14 @@
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -889,11 +925,14 @@
       <c r="C10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>1</v>
       </c>
@@ -903,11 +942,14 @@
       <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>2</v>
       </c>
@@ -917,11 +959,14 @@
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>2</v>
       </c>
@@ -931,11 +976,14 @@
       <c r="C13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>2</v>
       </c>
@@ -945,11 +993,14 @@
       <c r="C14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>2</v>
       </c>
@@ -959,11 +1010,14 @@
       <c r="C15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>2</v>
       </c>
@@ -973,11 +1027,14 @@
       <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>2</v>
       </c>
@@ -987,11 +1044,14 @@
       <c r="C17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>2</v>
       </c>
@@ -1001,11 +1061,14 @@
       <c r="C18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>2</v>
       </c>
@@ -1015,11 +1078,14 @@
       <c r="C19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>3</v>
       </c>
@@ -1029,11 +1095,14 @@
       <c r="C20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>3</v>
       </c>
@@ -1043,11 +1112,14 @@
       <c r="C21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>3</v>
       </c>
@@ -1057,11 +1129,14 @@
       <c r="C22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>4</v>
       </c>
@@ -1071,11 +1146,14 @@
       <c r="C23" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>4</v>
       </c>
@@ -1085,11 +1163,14 @@
       <c r="C24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>4</v>
       </c>
@@ -1099,11 +1180,14 @@
       <c r="C25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>4</v>
       </c>
@@ -1113,11 +1197,14 @@
       <c r="C26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>5</v>
       </c>
@@ -1127,11 +1214,14 @@
       <c r="C27" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>5</v>
       </c>
@@ -1141,11 +1231,14 @@
       <c r="C28" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>5</v>
       </c>
@@ -1155,11 +1248,14 @@
       <c r="C29" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>5</v>
       </c>
@@ -1169,11 +1265,14 @@
       <c r="C30" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>6</v>
       </c>
@@ -1183,11 +1282,14 @@
       <c r="C31" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>6</v>
       </c>
@@ -1197,11 +1299,14 @@
       <c r="C32" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>6</v>
       </c>
@@ -1211,11 +1316,14 @@
       <c r="C33" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>6</v>
       </c>
@@ -1225,11 +1333,14 @@
       <c r="C34" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>6</v>
       </c>
@@ -1239,11 +1350,14 @@
       <c r="C35" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>6</v>
       </c>
@@ -1253,11 +1367,14 @@
       <c r="C36" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>6</v>
       </c>
@@ -1267,11 +1384,14 @@
       <c r="C37" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>6</v>
       </c>
@@ -1281,11 +1401,14 @@
       <c r="C38" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>6</v>
       </c>
@@ -1295,11 +1418,14 @@
       <c r="C39" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>7</v>
       </c>
@@ -1309,11 +1435,14 @@
       <c r="C40" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>7</v>
       </c>
@@ -1323,11 +1452,14 @@
       <c r="C41" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>7</v>
       </c>
@@ -1337,11 +1469,14 @@
       <c r="C42" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>7</v>
       </c>
@@ -1351,11 +1486,14 @@
       <c r="C43" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>7</v>
       </c>
@@ -1365,11 +1503,14 @@
       <c r="C44" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>7</v>
       </c>
@@ -1379,11 +1520,14 @@
       <c r="C45" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>7</v>
       </c>
@@ -1393,11 +1537,14 @@
       <c r="C46" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>7</v>
       </c>
@@ -1407,11 +1554,14 @@
       <c r="C47" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>7</v>
       </c>
@@ -1421,11 +1571,14 @@
       <c r="C48" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>7</v>
       </c>
@@ -1435,11 +1588,14 @@
       <c r="C49" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>8</v>
       </c>
@@ -1449,11 +1605,14 @@
       <c r="C50" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>8</v>
       </c>
@@ -1463,11 +1622,14 @@
       <c r="C51" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>8</v>
       </c>
@@ -1477,11 +1639,14 @@
       <c r="C52" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>8</v>
       </c>
@@ -1491,11 +1656,14 @@
       <c r="C53" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>8</v>
       </c>
@@ -1505,11 +1673,14 @@
       <c r="C54" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>8</v>
       </c>
@@ -1519,11 +1690,14 @@
       <c r="C55" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>8</v>
       </c>
@@ -1533,11 +1707,14 @@
       <c r="C56" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>8</v>
       </c>
@@ -1547,11 +1724,14 @@
       <c r="C57" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D57" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>8</v>
       </c>
@@ -1561,11 +1741,14 @@
       <c r="C58" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D58" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>8</v>
       </c>
@@ -1575,11 +1758,14 @@
       <c r="C59" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D59" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>8</v>
       </c>
@@ -1589,11 +1775,14 @@
       <c r="C60" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D60" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>8</v>
       </c>
@@ -1603,11 +1792,14 @@
       <c r="C61" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D61" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>8</v>
       </c>
@@ -1617,11 +1809,14 @@
       <c r="C62" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D62" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>8</v>
       </c>
@@ -1631,11 +1826,14 @@
       <c r="C63" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D63" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>8</v>
       </c>
@@ -1645,11 +1843,14 @@
       <c r="C64" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D64" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>8</v>
       </c>
@@ -1659,11 +1860,14 @@
       <c r="C65" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D65" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E65" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>9</v>
       </c>
@@ -1673,11 +1877,14 @@
       <c r="C66" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D66" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>9</v>
       </c>
@@ -1687,11 +1894,14 @@
       <c r="C67" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D67" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>9</v>
       </c>
@@ -1701,11 +1911,14 @@
       <c r="C68" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D68" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E68" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>9</v>
       </c>
@@ -1715,11 +1928,14 @@
       <c r="C69" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="D69" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>9</v>
       </c>
@@ -1729,11 +1945,14 @@
       <c r="C70" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D70" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E70" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>9</v>
       </c>
@@ -1743,11 +1962,14 @@
       <c r="C71" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="D71" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E71" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>9</v>
       </c>
@@ -1757,11 +1979,14 @@
       <c r="C72" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D72" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E72" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>9</v>
       </c>
@@ -1771,11 +1996,14 @@
       <c r="C73" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D73" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E73" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>9</v>
       </c>
@@ -1785,11 +2013,14 @@
       <c r="C74" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D74" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>9</v>
       </c>
@@ -1799,11 +2030,14 @@
       <c r="C75" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="D75" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E75" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>9</v>
       </c>
@@ -1813,11 +2047,14 @@
       <c r="C76" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="D76" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E76" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>9</v>
       </c>
@@ -1827,11 +2064,14 @@
       <c r="C77" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D77" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E77" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>10</v>
       </c>
@@ -1841,11 +2081,14 @@
       <c r="C78" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="D78" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E78" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>10</v>
       </c>
@@ -1855,11 +2098,14 @@
       <c r="C79" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="D79" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E79" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>10</v>
       </c>
@@ -1869,11 +2115,14 @@
       <c r="C80" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="D80" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E80" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>10</v>
       </c>
@@ -1883,11 +2132,14 @@
       <c r="C81" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="D81" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E81" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>10</v>
       </c>
@@ -1897,11 +2149,14 @@
       <c r="C82" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="D82" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E82" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>10</v>
       </c>
@@ -1911,11 +2166,14 @@
       <c r="C83" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="D83" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E83" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>10</v>
       </c>
@@ -1925,11 +2183,14 @@
       <c r="C84" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="D84" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E84" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>10</v>
       </c>
@@ -1939,11 +2200,14 @@
       <c r="C85" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D85" s="1" t="s">
+      <c r="D85" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E85" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>11</v>
       </c>
@@ -1953,11 +2217,14 @@
       <c r="C86" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D86" s="1" t="s">
+      <c r="D86" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E86" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>11</v>
       </c>
@@ -1967,11 +2234,14 @@
       <c r="C87" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="D87" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>11</v>
       </c>
@@ -1981,11 +2251,14 @@
       <c r="C88" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="D88" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E88" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>11</v>
       </c>
@@ -1995,11 +2268,14 @@
       <c r="C89" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="D89" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E89" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>11</v>
       </c>
@@ -2009,11 +2285,14 @@
       <c r="C90" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="D90" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E90" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <v>11</v>
       </c>
@@ -2023,11 +2302,14 @@
       <c r="C91" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="D91" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E91" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>11</v>
       </c>
@@ -2037,11 +2319,14 @@
       <c r="C92" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D92" s="1" t="s">
+      <c r="D92" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E92" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>11</v>
       </c>
@@ -2051,11 +2336,14 @@
       <c r="C93" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D93" s="1" t="s">
+      <c r="D93" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E93" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>11</v>
       </c>
@@ -2065,11 +2353,14 @@
       <c r="C94" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D94" s="1" t="s">
+      <c r="D94" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E94" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>11</v>
       </c>
@@ -2079,11 +2370,14 @@
       <c r="C95" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D95" s="1" t="s">
+      <c r="D95" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E95" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>11</v>
       </c>
@@ -2093,11 +2387,14 @@
       <c r="C96" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="D96" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E96" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>11</v>
       </c>
@@ -2107,11 +2404,14 @@
       <c r="C97" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D97" s="1" t="s">
+      <c r="D97" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E97" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>12</v>
       </c>
@@ -2121,11 +2421,14 @@
       <c r="C98" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D98" s="1" t="s">
+      <c r="D98" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E98" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>12</v>
       </c>
@@ -2135,11 +2438,14 @@
       <c r="C99" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="D99" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E99" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>12</v>
       </c>
@@ -2149,11 +2455,14 @@
       <c r="C100" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D100" s="1" t="s">
+      <c r="D100" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E100" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>12</v>
       </c>
@@ -2163,11 +2472,14 @@
       <c r="C101" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D101" s="1" t="s">
+      <c r="D101" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E101" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>12</v>
       </c>
@@ -2177,11 +2489,14 @@
       <c r="C102" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D102" s="1" t="s">
+      <c r="D102" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E102" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <v>12</v>
       </c>
@@ -2191,11 +2506,14 @@
       <c r="C103" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D103" s="1" t="s">
+      <c r="D103" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E103" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>12</v>
       </c>
@@ -2205,11 +2523,14 @@
       <c r="C104" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D104" s="1" t="s">
+      <c r="D104" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E104" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <v>12</v>
       </c>
@@ -2219,11 +2540,14 @@
       <c r="C105" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D105" s="1" t="s">
+      <c r="D105" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E105" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <v>12</v>
       </c>
@@ -2233,7 +2557,10 @@
       <c r="C106" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D106" s="1" t="s">
+      <c r="D106" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E106" s="1" t="s">
         <v>112</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added priorization of days
</commit_message>
<xml_diff>
--- a/data/special_days.xlsx
+++ b/data/special_days.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Manue\Documents\R Scripts\Catholic_Calendar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9BEAEE3-2DD5-4332-BB4B-0EE2D386F1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26889D19-8B43-4C7D-8970-4C53B9053600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{DB0BE976-C12D-413B-BEEB-3B29EA804A45}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="117">
   <si>
     <t>type</t>
   </si>
@@ -384,6 +384,9 @@
   </si>
   <si>
     <t>Exaltation of the Cross</t>
+  </si>
+  <si>
+    <t>Appearance of the Lord</t>
   </si>
 </sst>
 </file>
@@ -752,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AE50AD-9324-4F6C-B024-445672FDC880}">
   <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,6 +854,9 @@
       <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="F5" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4">

</xml_diff>